<commit_message>
inserito parte documentazione sphinx in src/docs
</commit_message>
<xml_diff>
--- a/input/input_elaborati/items.xlsx
+++ b/input/input_elaborati/items.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,7 +569,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" t="n">
         <v>22150309</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" t="n">
         <v>22215135</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B5" t="n">
         <v>22253240</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B6" t="n">
         <v>22264189</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B7" t="n">
         <v>22272792</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B8" t="n">
         <v>22274471</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B9" t="n">
         <v>22281682</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B10" t="n">
         <v>22303604</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B11" t="n">
         <v>23006411</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B12" t="n">
         <v>23008895</v>
@@ -1145,14 +1145,14 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B13" t="n">
-        <v>23008947</v>
+        <v>23008953</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LU2B 1501A</t>
+          <t>LU2D 0700</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>09/23</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1184,13 +1184,13 @@
         </is>
       </c>
       <c r="J13" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>180</v>
+        <v>128</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
@@ -1203,14 +1203,14 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>853</v>
+        <v>870</v>
       </c>
       <c r="B14" t="n">
-        <v>23008953</v>
+        <v>23008996</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LU2D 0700</t>
+          <t>LU2C 1500</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>09/23</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>128</v>
+        <v>311</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1261,32 +1261,32 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>856</v>
+        <v>933</v>
       </c>
       <c r="B15" t="n">
-        <v>23008956</v>
+        <v>23016975</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LU4B 0300</t>
+          <t>LU90M010</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>50</v>
+        <v>507</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1319,32 +1319,32 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>872</v>
+        <v>945</v>
       </c>
       <c r="B16" t="n">
-        <v>23008996</v>
+        <v>23017009</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LU2C 1500</t>
+          <t>D200MD08LH</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>50</v>
+        <v>501</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>311</v>
+        <v>250</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
@@ -1377,14 +1377,14 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>935</v>
+        <v>947</v>
       </c>
       <c r="B17" t="n">
-        <v>23016975</v>
+        <v>23017011</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LU90M010</t>
+          <t>D200MD08LH</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1394,11 +1394,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>95</v>
+        <v>250</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
@@ -1435,14 +1435,14 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>947</v>
+        <v>952</v>
       </c>
       <c r="B18" t="n">
-        <v>23017009</v>
+        <v>23017016</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>D200MD08LH</t>
+          <t>D200MD08RH</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1460,7 +1460,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1493,14 +1493,14 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>949</v>
+        <v>1009</v>
       </c>
       <c r="B19" t="n">
-        <v>23017011</v>
+        <v>23017154</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>D200MD08LH</t>
+          <t>LU2F 0600B</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1510,15 +1510,15 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1532,13 +1532,13 @@
         </is>
       </c>
       <c r="J19" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>250</v>
+        <v>72</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
@@ -1551,14 +1551,14 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>954</v>
+        <v>1039</v>
       </c>
       <c r="B20" t="n">
-        <v>23017016</v>
+        <v>23019356</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>D200MD08RH</t>
+          <t>LCL7M10010</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1568,15 +1568,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>501</v>
+        <v>50</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1590,13 +1590,13 @@
         </is>
       </c>
       <c r="J20" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>250</v>
+        <v>31</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -1609,28 +1609,28 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1011</v>
+        <v>1062</v>
       </c>
       <c r="B21" t="n">
-        <v>23017154</v>
+        <v>23019400</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LU2F 0600B</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>505</v>
+        <v>50</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1648,13 +1648,13 @@
         </is>
       </c>
       <c r="J21" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
@@ -1667,14 +1667,14 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1041</v>
+        <v>1063</v>
       </c>
       <c r="B22" t="n">
-        <v>23019356</v>
+        <v>23019401</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LCL7M10010</t>
+          <t>LU1A 0200</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1706,13 +1706,13 @@
         </is>
       </c>
       <c r="J22" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
@@ -1728,21 +1728,21 @@
         <v>1064</v>
       </c>
       <c r="B23" t="n">
-        <v>23019400</v>
+        <v>23019405</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>LU1H 1101</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1764,13 +1764,13 @@
         </is>
       </c>
       <c r="J23" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
@@ -1783,19 +1783,19 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B24" t="n">
-        <v>23019401</v>
+        <v>23019416</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LU1A 0200</t>
+          <t>LU3D 1500</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1828,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>34</v>
+        <v>240</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
@@ -1841,24 +1841,24 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="B25" t="n">
-        <v>23019405</v>
+        <v>23019418</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LU1H 1101</t>
+          <t>LU3F 0300</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1880,13 +1880,13 @@
         </is>
       </c>
       <c r="J25" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>48</v>
+        <v>480</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
@@ -1899,14 +1899,14 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1068</v>
+        <v>1097</v>
       </c>
       <c r="B26" t="n">
-        <v>23019416</v>
+        <v>23019464</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LU3D 1500</t>
+          <t>LA92MT 001</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="J26" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>240</v>
+        <v>312</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
@@ -1957,14 +1957,14 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1070</v>
+        <v>1100</v>
       </c>
       <c r="B27" t="n">
-        <v>23019418</v>
+        <v>23019468</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LU3F 0300</t>
+          <t>LU2C 1500</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>480</v>
+        <v>312</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
@@ -2015,14 +2015,14 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="B28" t="n">
-        <v>23019464</v>
+        <v>23019470</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>LA92MT 001</t>
+          <t>LU3D 0400</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -2054,13 +2054,13 @@
         </is>
       </c>
       <c r="J28" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
@@ -2073,14 +2073,14 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1102</v>
+        <v>1355</v>
       </c>
       <c r="B29" t="n">
-        <v>23019468</v>
+        <v>23026450</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>LU2C 1500</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2112,13 +2112,13 @@
         </is>
       </c>
       <c r="J29" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>312</v>
+        <v>50</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
@@ -2131,32 +2131,32 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1104</v>
+        <v>1358</v>
       </c>
       <c r="B30" t="n">
-        <v>23019470</v>
+        <v>23026457</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>LU3D 0400</t>
+          <t>LENDM0842FX</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>50</v>
+        <v>503</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>320</v>
+        <v>419</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
@@ -2189,32 +2189,32 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1357</v>
+        <v>1362</v>
       </c>
       <c r="B31" t="n">
-        <v>23026450</v>
+        <v>23026466</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>LENDM1296NC</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>50</v>
+        <v>503</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>10/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2228,13 +2228,13 @@
         </is>
       </c>
       <c r="J31" s="2" t="n">
-        <v>44994</v>
+        <v>44992</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
@@ -2247,14 +2247,14 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1360</v>
+        <v>1374</v>
       </c>
       <c r="B32" t="n">
-        <v>23026457</v>
+        <v>23026485</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LENDM0842FX</t>
+          <t>LU91M250</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2264,15 +2264,15 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2292,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>419</v>
+        <v>97</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
@@ -2305,14 +2305,14 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1364</v>
+        <v>1379</v>
       </c>
       <c r="B33" t="n">
-        <v>23026466</v>
+        <v>23026504</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LENDM1296NC</t>
+          <t>LENDM1296N</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2350,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>180</v>
+        <v>324</v>
       </c>
       <c r="M33" t="inlineStr">
         <is>
@@ -2363,14 +2363,14 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1376</v>
+        <v>1380</v>
       </c>
       <c r="B34" t="n">
-        <v>23026485</v>
+        <v>23026505</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LU91M250</t>
+          <t>LENDM1296N</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2380,11 +2380,11 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>97</v>
+        <v>324</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
@@ -2424,7 +2424,7 @@
         <v>1381</v>
       </c>
       <c r="B35" t="n">
-        <v>23026504</v>
+        <v>23026506</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2460,7 +2460,7 @@
         </is>
       </c>
       <c r="J35" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K35" t="n">
         <v>0</v>
@@ -2479,14 +2479,14 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>1382</v>
+        <v>1386</v>
       </c>
       <c r="B36" t="n">
-        <v>23026505</v>
+        <v>23026511</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LENDM1296N</t>
+          <t>D200MD08LH</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2524,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>324</v>
+        <v>250</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
@@ -2537,14 +2537,14 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>1383</v>
+        <v>1389</v>
       </c>
       <c r="B37" t="n">
-        <v>23026506</v>
+        <v>23026514</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LENDM1296N</t>
+          <t>D200MD08RH</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2576,13 +2576,13 @@
         </is>
       </c>
       <c r="J37" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K37" t="n">
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>324</v>
+        <v>250</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
@@ -2595,14 +2595,14 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>1388</v>
+        <v>1393</v>
       </c>
       <c r="B38" t="n">
-        <v>23026511</v>
+        <v>23026907</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>D200MD08LH</t>
+          <t>BO2608642385</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2612,15 +2612,15 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2634,13 +2634,13 @@
         </is>
       </c>
       <c r="J38" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K38" t="n">
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>250</v>
+        <v>159</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
@@ -2653,14 +2653,14 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>1391</v>
+        <v>1421</v>
       </c>
       <c r="B39" t="n">
-        <v>23026514</v>
+        <v>23026961</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>D200MD08RH</t>
+          <t>LU2F 0201B</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2670,15 +2670,15 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2692,13 +2692,13 @@
         </is>
       </c>
       <c r="J39" s="2" t="n">
-        <v>44994</v>
+        <v>44992</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>250</v>
+        <v>346</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
@@ -2711,28 +2711,28 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>1395</v>
+        <v>1446</v>
       </c>
       <c r="B40" t="n">
-        <v>23026907</v>
+        <v>23028523</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BO2608642385</t>
+          <t>LI25M31EB3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>505</v>
+        <v>50</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2750,13 +2750,13 @@
         </is>
       </c>
       <c r="J40" s="2" t="n">
-        <v>44994</v>
+        <v>44992</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>159</v>
+        <v>320</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
@@ -2769,19 +2769,19 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1423</v>
+        <v>1477</v>
       </c>
       <c r="B41" t="n">
-        <v>23026961</v>
+        <v>23028565</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LU2F 0201B</t>
+          <t>LU2B 0701</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2790,11 +2790,11 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>505</v>
+        <v>50</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2814,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>346</v>
+        <v>40</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
@@ -2827,14 +2827,14 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>1448</v>
+        <v>1479</v>
       </c>
       <c r="B42" t="n">
-        <v>23028523</v>
+        <v>23028568</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>LI25M31EB3</t>
+          <t>LU2C 1200</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2866,13 +2866,13 @@
         </is>
       </c>
       <c r="J42" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>320</v>
+        <v>254</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -2885,14 +2885,14 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="B43" t="n">
-        <v>23028565</v>
+        <v>23028570</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>LU2B 0701</t>
+          <t>LU2C 1901A</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2924,13 +2924,13 @@
         </is>
       </c>
       <c r="J43" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K43" t="n">
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -2943,14 +2943,14 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1481</v>
+        <v>1504</v>
       </c>
       <c r="B44" t="n">
-        <v>23028568</v>
+        <v>23028598</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>LU2C 1200</t>
+          <t>LA92MT 001</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2988,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
@@ -3001,14 +3001,14 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1482</v>
+        <v>1505</v>
       </c>
       <c r="B45" t="n">
-        <v>23028570</v>
+        <v>23028599</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LU2C 1901A</t>
+          <t>LA92MT 001</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3046,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>108</v>
+        <v>312</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
@@ -3059,19 +3059,19 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1494</v>
+        <v>1511</v>
       </c>
       <c r="B46" t="n">
-        <v>23028583</v>
+        <v>23028606</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PLS0000024</t>
+          <t>PLS0000035</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -3098,13 +3098,13 @@
         </is>
       </c>
       <c r="J46" s="2" t="n">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
@@ -3117,19 +3117,19 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>1506</v>
+        <v>1512</v>
       </c>
       <c r="B47" t="n">
-        <v>23028598</v>
+        <v>23028607</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>LA92MT 001</t>
+          <t>PLS0000035</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3162,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>312</v>
+        <v>240</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
@@ -3175,19 +3175,19 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1507</v>
+        <v>1513</v>
       </c>
       <c r="B48" t="n">
-        <v>23028599</v>
+        <v>23028608</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>LA92MT 001</t>
+          <t>PLS0000035</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>11/23</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3214,13 +3214,13 @@
         </is>
       </c>
       <c r="J48" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K48" t="n">
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>312</v>
+        <v>160</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
@@ -3233,24 +3233,24 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1513</v>
+        <v>1521</v>
       </c>
       <c r="B49" t="n">
-        <v>23028606</v>
+        <v>23029690</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PLS0000035</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3272,13 +3272,13 @@
         </is>
       </c>
       <c r="J49" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K49" t="n">
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>237</v>
+        <v>54</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
@@ -3291,24 +3291,24 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>1514</v>
+        <v>1522</v>
       </c>
       <c r="B50" t="n">
-        <v>23028607</v>
+        <v>23029691</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PLS0000035</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3330,13 +3330,13 @@
         </is>
       </c>
       <c r="J50" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>240</v>
+        <v>54</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
@@ -3349,24 +3349,24 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>1515</v>
+        <v>1526</v>
       </c>
       <c r="B51" t="n">
-        <v>23028608</v>
+        <v>23030009</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>PLS0000035</t>
+          <t>LI25M28EB3</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3388,13 +3388,13 @@
         </is>
       </c>
       <c r="J51" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K51" t="n">
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>160</v>
+        <v>648</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
@@ -3407,14 +3407,14 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>1520</v>
+        <v>1560</v>
       </c>
       <c r="B52" t="n">
-        <v>23028656</v>
+        <v>23037502</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>LU82M  CA3</t>
+          <t>LENDP1040UX</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -3424,15 +3424,15 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>11/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3446,13 +3446,13 @@
         </is>
       </c>
       <c r="J52" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K52" t="n">
         <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>64</v>
+        <v>326</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
@@ -3465,19 +3465,19 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>1523</v>
+        <v>1606</v>
       </c>
       <c r="B53" t="n">
-        <v>23029690</v>
+        <v>23037566</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>FSTL000001</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -3486,11 +3486,11 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>50</v>
+        <v>521</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3504,13 +3504,13 @@
         </is>
       </c>
       <c r="J53" s="2" t="n">
-        <v>44994</v>
+        <v>44991</v>
       </c>
       <c r="K53" t="n">
         <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>54</v>
+        <v>288</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
@@ -3523,19 +3523,19 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>1524</v>
+        <v>1607</v>
       </c>
       <c r="B54" t="n">
-        <v>23029691</v>
+        <v>23037567</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>FSTL000001</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -3544,11 +3544,11 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>50</v>
+        <v>521</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3562,13 +3562,13 @@
         </is>
       </c>
       <c r="J54" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K54" t="n">
         <v>0</v>
       </c>
       <c r="L54" t="n">
-        <v>54</v>
+        <v>288</v>
       </c>
       <c r="M54" t="inlineStr">
         <is>
@@ -3581,19 +3581,19 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1528</v>
+        <v>1608</v>
       </c>
       <c r="B55" t="n">
-        <v>23030009</v>
+        <v>23037568</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LI25M28EB3</t>
+          <t>FSTL000001</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -3602,11 +3602,11 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>50</v>
+        <v>521</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3620,13 +3620,13 @@
         </is>
       </c>
       <c r="J55" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K55" t="n">
         <v>0</v>
       </c>
       <c r="L55" t="n">
-        <v>648</v>
+        <v>287</v>
       </c>
       <c r="M55" t="inlineStr">
         <is>
@@ -3639,14 +3639,14 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>1562</v>
+        <v>1609</v>
       </c>
       <c r="B56" t="n">
-        <v>23037502</v>
+        <v>23037569</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>LENDP1040UX</t>
+          <t>FSTL000001</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3656,11 +3656,11 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="L56" t="n">
-        <v>326</v>
+        <v>285</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
@@ -3697,32 +3697,32 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>1608</v>
+        <v>1676</v>
       </c>
       <c r="B57" t="n">
-        <v>23037566</v>
+        <v>23040776</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>FSTL000001</t>
+          <t>FR06F001H</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>521</v>
+        <v>50</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3736,17 +3736,17 @@
         </is>
       </c>
       <c r="J57" s="2" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="K57" t="n">
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>288</v>
+        <v>216</v>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>450 300 AFFILATURA LAME</t>
+          <t>528 391 LAVAGGIO E CONTROLLO</t>
         </is>
       </c>
       <c r="N57" t="n">
@@ -3755,14 +3755,14 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>1609</v>
+        <v>1692</v>
       </c>
       <c r="B58" t="n">
-        <v>23037567</v>
+        <v>23040802</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>FSTL000001</t>
+          <t>LCL7M10072</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3772,15 +3772,15 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>521</v>
+        <v>50</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="L58" t="n">
-        <v>288</v>
+        <v>60</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
@@ -3813,19 +3813,19 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>1610</v>
+        <v>1707</v>
       </c>
       <c r="B59" t="n">
-        <v>23037568</v>
+        <v>23040825</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>FSTL000001</t>
+          <t>LSB38004X</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -3834,11 +3834,11 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>521</v>
+        <v>50</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3858,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>287</v>
+        <v>50</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
@@ -3871,14 +3871,14 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1678</v>
+        <v>1717</v>
       </c>
       <c r="B60" t="n">
-        <v>23040776</v>
+        <v>23040840</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>FR06F001H</t>
+          <t>LU1I 0900</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -3910,17 +3910,17 @@
         </is>
       </c>
       <c r="J60" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K60" t="n">
         <v>0</v>
       </c>
       <c r="L60" t="n">
-        <v>216</v>
+        <v>90</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>528 391 LAVAGGIO E CONTROLLO</t>
+          <t>450 300 AFFILATURA LAME</t>
         </is>
       </c>
       <c r="N60" t="n">
@@ -3929,19 +3929,19 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>1694</v>
+        <v>1729</v>
       </c>
       <c r="B61" t="n">
-        <v>23040802</v>
+        <v>23040853</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>LCL7M10072</t>
+          <t>LU3A 0001</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3968,13 +3968,13 @@
         </is>
       </c>
       <c r="J61" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K61" t="n">
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -3987,14 +3987,14 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>1709</v>
+        <v>1731</v>
       </c>
       <c r="B62" t="n">
-        <v>23040825</v>
+        <v>23040857</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LSB38004X</t>
+          <t>LU3D 0900</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -4012,7 +4012,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -4026,13 +4026,13 @@
         </is>
       </c>
       <c r="J62" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K62" t="n">
         <v>0</v>
       </c>
       <c r="L62" t="n">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
@@ -4045,14 +4045,14 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>1719</v>
+        <v>1738</v>
       </c>
       <c r="B63" t="n">
-        <v>23040840</v>
+        <v>23040869</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>LU1I 0900</t>
+          <t>LU5D 0800</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -4084,13 +4084,13 @@
         </is>
       </c>
       <c r="J63" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K63" t="n">
         <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>90</v>
+        <v>224</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
@@ -4103,14 +4103,14 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1731</v>
+        <v>1769</v>
       </c>
       <c r="B64" t="n">
-        <v>23040853</v>
+        <v>23040992</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>LU3A 0001</t>
+          <t>LI25M31EA3</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -4148,7 +4148,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>214</v>
+        <v>640</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
@@ -4161,14 +4161,14 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>1733</v>
+        <v>1770</v>
       </c>
       <c r="B65" t="n">
-        <v>23040857</v>
+        <v>23040993</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>LU3D 0900</t>
+          <t>LI25M31EA3</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -4186,7 +4186,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>12/23</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -4200,13 +4200,13 @@
         </is>
       </c>
       <c r="J65" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K65" t="n">
         <v>0</v>
       </c>
       <c r="L65" t="n">
-        <v>176</v>
+        <v>640</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
@@ -4219,14 +4219,14 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>1740</v>
+        <v>1774</v>
       </c>
       <c r="B66" t="n">
-        <v>23040869</v>
+        <v>23040997</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LU5D 0800</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -4244,7 +4244,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4258,13 +4258,13 @@
         </is>
       </c>
       <c r="J66" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K66" t="n">
         <v>0</v>
       </c>
       <c r="L66" t="n">
-        <v>224</v>
+        <v>49</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
@@ -4277,14 +4277,14 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>1771</v>
+        <v>1775</v>
       </c>
       <c r="B67" t="n">
-        <v>23040992</v>
+        <v>23040998</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LI25M31EA3</t>
+          <t>LU3D 0400</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -4316,13 +4316,13 @@
         </is>
       </c>
       <c r="J67" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K67" t="n">
         <v>0</v>
       </c>
       <c r="L67" t="n">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
@@ -4335,24 +4335,24 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1772</v>
+        <v>1806</v>
       </c>
       <c r="B68" t="n">
-        <v>23040993</v>
+        <v>23043403</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>LI25M31EA3</t>
+          <t>LCCAM3D0970</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>  </t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4374,13 +4374,13 @@
         </is>
       </c>
       <c r="J68" s="2" t="n">
-        <v>44994</v>
+        <v>44984</v>
       </c>
       <c r="K68" t="n">
         <v>0</v>
       </c>
       <c r="L68" t="n">
-        <v>640</v>
+        <v>12</v>
       </c>
       <c r="M68" t="inlineStr">
         <is>
@@ -4393,28 +4393,28 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>1776</v>
+        <v>1916</v>
       </c>
       <c r="B69" t="n">
-        <v>23040997</v>
+        <v>23048848</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>LENDP053830FM</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>50</v>
+        <v>501</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="L69" t="n">
-        <v>49</v>
+        <v>672</v>
       </c>
       <c r="M69" t="inlineStr">
         <is>
@@ -4451,32 +4451,32 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>1777</v>
+        <v>1922</v>
       </c>
       <c r="B70" t="n">
-        <v>23040998</v>
+        <v>23048855</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>LU3D 0400</t>
+          <t>LM71M  CA3</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>50</v>
+        <v>507</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>12/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -4496,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="L70" t="n">
-        <v>320</v>
+        <v>55</v>
       </c>
       <c r="M70" t="inlineStr">
         <is>
@@ -4509,32 +4509,32 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>1808</v>
+        <v>1927</v>
       </c>
       <c r="B71" t="n">
-        <v>23043403</v>
+        <v>23048860</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>LCCAM3D0970</t>
+          <t>LU74MR FA3</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>  </t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>EA</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>50</v>
+        <v>507</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4548,13 +4548,13 @@
         </is>
       </c>
       <c r="J71" s="2" t="n">
-        <v>44984</v>
+        <v>44994</v>
       </c>
       <c r="K71" t="n">
         <v>0</v>
       </c>
       <c r="L71" t="n">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="M71" t="inlineStr">
         <is>
@@ -4567,14 +4567,14 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>1919</v>
+        <v>2001</v>
       </c>
       <c r="B72" t="n">
-        <v>23048848</v>
+        <v>23050584</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>LENDP053830FM</t>
+          <t>BO2608644013</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -4584,15 +4584,15 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -4606,13 +4606,13 @@
         </is>
       </c>
       <c r="J72" s="2" t="n">
-        <v>44994</v>
+        <v>44991</v>
       </c>
       <c r="K72" t="n">
         <v>0</v>
       </c>
       <c r="L72" t="n">
-        <v>672</v>
+        <v>102</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
@@ -4625,14 +4625,14 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>1925</v>
+        <v>2021</v>
       </c>
       <c r="B73" t="n">
-        <v>23048855</v>
+        <v>23050604</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LM71M  CA3</t>
+          <t>BO2608644062</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -4642,11 +4642,11 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -4664,13 +4664,13 @@
         </is>
       </c>
       <c r="J73" s="2" t="n">
-        <v>44993</v>
+        <v>44991</v>
       </c>
       <c r="K73" t="n">
         <v>0</v>
       </c>
       <c r="L73" t="n">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="M73" t="inlineStr">
         <is>
@@ -4683,32 +4683,32 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>1930</v>
+        <v>2080</v>
       </c>
       <c r="B74" t="n">
-        <v>23048860</v>
+        <v>23052633</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LU74MR FA3</t>
+          <t>FR04A001H</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>507</v>
+        <v>50</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>14/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4722,13 +4722,13 @@
         </is>
       </c>
       <c r="J74" s="2" t="n">
-        <v>44994</v>
+        <v>44986</v>
       </c>
       <c r="K74" t="n">
         <v>0</v>
       </c>
       <c r="L74" t="n">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
@@ -4741,19 +4741,19 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>2004</v>
+        <v>2090</v>
       </c>
       <c r="B75" t="n">
-        <v>23050584</v>
+        <v>23052644</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BO2608644013</t>
+          <t>FR07W009HC</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -4762,7 +4762,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>505</v>
+        <v>50</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -4780,13 +4780,13 @@
         </is>
       </c>
       <c r="J75" s="2" t="n">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="K75" t="n">
         <v>0</v>
       </c>
       <c r="L75" t="n">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
@@ -4799,19 +4799,19 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>2024</v>
+        <v>2126</v>
       </c>
       <c r="B76" t="n">
-        <v>23050604</v>
+        <v>23052689</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BO2608644062</t>
+          <t>LI25M31003</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -4820,11 +4820,11 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>505</v>
+        <v>50</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>14/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4838,13 +4838,13 @@
         </is>
       </c>
       <c r="J76" s="2" t="n">
-        <v>44991</v>
+        <v>44992</v>
       </c>
       <c r="K76" t="n">
         <v>0</v>
       </c>
       <c r="L76" t="n">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
@@ -4857,14 +4857,14 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>2083</v>
+        <v>2127</v>
       </c>
       <c r="B77" t="n">
-        <v>23052633</v>
+        <v>23052690</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FR04A001H</t>
+          <t>LI25M43KE3</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -4874,7 +4874,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -4896,13 +4896,13 @@
         </is>
       </c>
       <c r="J77" s="2" t="n">
-        <v>44986</v>
+        <v>44992</v>
       </c>
       <c r="K77" t="n">
         <v>0</v>
       </c>
       <c r="L77" t="n">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
@@ -4915,14 +4915,14 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>2093</v>
+        <v>2128</v>
       </c>
       <c r="B78" t="n">
-        <v>23052644</v>
+        <v>23052691</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>FR07W009HC</t>
+          <t>LI25M43LG3</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F78" t="n">
@@ -4960,7 +4960,7 @@
         <v>0</v>
       </c>
       <c r="L78" t="n">
-        <v>32</v>
+        <v>215</v>
       </c>
       <c r="M78" t="inlineStr">
         <is>
@@ -4973,14 +4973,14 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>2129</v>
+        <v>2132</v>
       </c>
       <c r="B79" t="n">
-        <v>23052689</v>
+        <v>23052695</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>LI25M31003</t>
+          <t>LI25M47NE3</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F79" t="n">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -5012,13 +5012,13 @@
         </is>
       </c>
       <c r="J79" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K79" t="n">
         <v>0</v>
       </c>
       <c r="L79" t="n">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
@@ -5031,14 +5031,14 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>2130</v>
+        <v>2154</v>
       </c>
       <c r="B80" t="n">
-        <v>23052690</v>
+        <v>23052722</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>LI25M43KE3</t>
+          <t>LU1C 0100</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -5070,13 +5070,13 @@
         </is>
       </c>
       <c r="J80" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K80" t="n">
         <v>0</v>
       </c>
       <c r="L80" t="n">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
@@ -5089,14 +5089,14 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>2131</v>
+        <v>2167</v>
       </c>
       <c r="B81" t="n">
-        <v>23052691</v>
+        <v>23052737</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LI25M43LG3</t>
+          <t>LU2B 0300</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -5114,7 +5114,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>14/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -5128,13 +5128,13 @@
         </is>
       </c>
       <c r="J81" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K81" t="n">
         <v>0</v>
       </c>
       <c r="L81" t="n">
-        <v>215</v>
+        <v>100</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
@@ -5147,14 +5147,14 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>2135</v>
+        <v>2168</v>
       </c>
       <c r="B82" t="n">
-        <v>23052695</v>
+        <v>23052738</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LI25M47NE3</t>
+          <t>LU2B 0500</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -5172,7 +5172,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>14/23</t>
+          <t>13/23</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -5192,7 +5192,7 @@
         <v>0</v>
       </c>
       <c r="L82" t="n">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
@@ -5205,19 +5205,19 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>2157</v>
+        <v>2175</v>
       </c>
       <c r="B83" t="n">
-        <v>23052722</v>
+        <v>23052745</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>LU1C 0100</t>
+          <t>LU2C 1201</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -5250,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
@@ -5263,14 +5263,14 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>2170</v>
+        <v>2184</v>
       </c>
       <c r="B84" t="n">
-        <v>23052737</v>
+        <v>23052754</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>LU2B 0300</t>
+          <t>LU3E 0200</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -5308,7 +5308,7 @@
         <v>0</v>
       </c>
       <c r="L84" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
@@ -5321,14 +5321,14 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>2171</v>
+        <v>2187</v>
       </c>
       <c r="B85" t="n">
-        <v>23052738</v>
+        <v>23052757</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>LU2B 0500</t>
+          <t>LU4B 0100</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -5360,13 +5360,13 @@
         </is>
       </c>
       <c r="J85" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K85" t="n">
         <v>0</v>
       </c>
       <c r="L85" t="n">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
@@ -5379,14 +5379,14 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>2178</v>
+        <v>2200</v>
       </c>
       <c r="B86" t="n">
-        <v>23052745</v>
+        <v>23052770</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>LU2C 1201</t>
+          <t>GL20702ML</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -5396,7 +5396,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -5418,13 +5418,13 @@
         </is>
       </c>
       <c r="J86" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K86" t="n">
         <v>0</v>
       </c>
       <c r="L86" t="n">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
@@ -5437,24 +5437,24 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>2187</v>
+        <v>2201</v>
       </c>
       <c r="B87" t="n">
-        <v>23052754</v>
+        <v>23052771</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>LU3E 0200</t>
+          <t>GL20702MR</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -5476,13 +5476,13 @@
         </is>
       </c>
       <c r="J87" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K87" t="n">
         <v>0</v>
       </c>
       <c r="L87" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M87" t="inlineStr">
         <is>
@@ -5495,24 +5495,24 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>2190</v>
+        <v>2203</v>
       </c>
       <c r="B88" t="n">
-        <v>23052757</v>
+        <v>23052773</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>LU4B 0100</t>
+          <t>GL20702M32</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EV</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -5534,13 +5534,13 @@
         </is>
       </c>
       <c r="J88" s="2" t="n">
-        <v>44993</v>
+        <v>44992</v>
       </c>
       <c r="K88" t="n">
         <v>0</v>
       </c>
       <c r="L88" t="n">
-        <v>49</v>
+        <v>224</v>
       </c>
       <c r="M88" t="inlineStr">
         <is>
@@ -5553,24 +5553,24 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>2203</v>
+        <v>2209</v>
       </c>
       <c r="B89" t="n">
-        <v>23052770</v>
+        <v>23052828</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>GL20702ML</t>
+          <t>FR07W012HC</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F89" t="n">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -5592,13 +5592,13 @@
         </is>
       </c>
       <c r="J89" s="2" t="n">
-        <v>44992</v>
+        <v>44993</v>
       </c>
       <c r="K89" t="n">
         <v>0</v>
       </c>
       <c r="L89" t="n">
-        <v>54</v>
+        <v>354</v>
       </c>
       <c r="M89" t="inlineStr">
         <is>
@@ -5611,24 +5611,24 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>2204</v>
+        <v>2223</v>
       </c>
       <c r="B90" t="n">
-        <v>23052771</v>
+        <v>23052844</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>GL20702MR</t>
+          <t>LSB45017X</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -5650,13 +5650,13 @@
         </is>
       </c>
       <c r="J90" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K90" t="n">
         <v>0</v>
       </c>
       <c r="L90" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
@@ -5669,24 +5669,24 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>2206</v>
+        <v>2226</v>
       </c>
       <c r="B91" t="n">
-        <v>23052773</v>
+        <v>23052917</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>GL20702M32</t>
+          <t>LL02M20060</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>EV</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -5708,13 +5708,13 @@
         </is>
       </c>
       <c r="J91" s="2" t="n">
-        <v>44992</v>
+        <v>44994</v>
       </c>
       <c r="K91" t="n">
         <v>0</v>
       </c>
       <c r="L91" t="n">
-        <v>224</v>
+        <v>31</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
@@ -5727,28 +5727,28 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>2212</v>
+        <v>2360</v>
       </c>
       <c r="B92" t="n">
-        <v>23052828</v>
+        <v>23059571</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>FR07W012HC</t>
+          <t>LENDM0516X</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>DM</t>
+          <t>FA</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>50</v>
+        <v>501</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -5766,13 +5766,13 @@
         </is>
       </c>
       <c r="J92" s="2" t="n">
-        <v>44993</v>
+        <v>44994</v>
       </c>
       <c r="K92" t="n">
         <v>0</v>
       </c>
       <c r="L92" t="n">
-        <v>354</v>
+        <v>299</v>
       </c>
       <c r="M92" t="inlineStr">
         <is>
@@ -5785,32 +5785,32 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>2226</v>
+        <v>2390</v>
       </c>
       <c r="B93" t="n">
-        <v>23052844</v>
+        <v>23059608</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>LSB45017X</t>
+          <t>LU89M  IA3</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>50</v>
+        <v>507</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5824,13 +5824,13 @@
         </is>
       </c>
       <c r="J93" s="2" t="n">
-        <v>44994</v>
+        <v>44993</v>
       </c>
       <c r="K93" t="n">
         <v>0</v>
       </c>
       <c r="L93" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
@@ -5843,14 +5843,14 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>2229</v>
+        <v>2399</v>
       </c>
       <c r="B94" t="n">
-        <v>23052917</v>
+        <v>23062906</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>LL02M20060</t>
+          <t>FR16W002TC</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -5860,7 +5860,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>DH</t>
+          <t>DM</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>13/23</t>
+          <t>14/23</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -5888,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="L94" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="M94" t="inlineStr">
         <is>
@@ -5901,14 +5901,14 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>2363</v>
+        <v>2432</v>
       </c>
       <c r="B95" t="n">
-        <v>23059571</v>
+        <v>23062948</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>LENDM0516X</t>
+          <t>LP33M  MP3</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -5918,11 +5918,11 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>FA</t>
+          <t>DH</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>501</v>
+        <v>50</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -5946,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>299</v>
+        <v>30</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
@@ -5954,180 +5954,6 @@
         </is>
       </c>
       <c r="N95" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>2393</v>
-      </c>
-      <c r="B96" t="n">
-        <v>23059608</v>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>LU89M  IA3</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>MO</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>EG</t>
-        </is>
-      </c>
-      <c r="F96" t="n">
-        <v>507</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>14/23</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>TRASF. IN AFFILATURA</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="J96" s="2" t="n">
-        <v>44993</v>
-      </c>
-      <c r="K96" t="n">
-        <v>0</v>
-      </c>
-      <c r="L96" t="n">
-        <v>55</v>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>450 300 AFFILATURA LAME</t>
-        </is>
-      </c>
-      <c r="N96" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>2402</v>
-      </c>
-      <c r="B97" t="n">
-        <v>23062906</v>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>FR16W002TC</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>DM</t>
-        </is>
-      </c>
-      <c r="F97" t="n">
-        <v>50</v>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>14/23</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>TRASF. IN AFFILATURA</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="J97" s="2" t="n">
-        <v>44994</v>
-      </c>
-      <c r="K97" t="n">
-        <v>0</v>
-      </c>
-      <c r="L97" t="n">
-        <v>50</v>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>450 300 AFFILATURA LAME</t>
-        </is>
-      </c>
-      <c r="N97" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>2435</v>
-      </c>
-      <c r="B98" t="n">
-        <v>23062948</v>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>LP33M  MP3</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>MO</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>DH</t>
-        </is>
-      </c>
-      <c r="F98" t="n">
-        <v>50</v>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>14/23</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>TRASF. IN AFFILATURA</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="J98" s="2" t="n">
-        <v>44994</v>
-      </c>
-      <c r="K98" t="n">
-        <v>0</v>
-      </c>
-      <c r="L98" t="n">
-        <v>30</v>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>450 300 AFFILATURA LAME</t>
-        </is>
-      </c>
-      <c r="N98" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>